<commit_message>
aggiornamento test accreditamento SynbrAIn srl
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#SYNBRAINSRLXX/SynbrAIn srl/AID Patient Summary/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#SYNBRAINSRLXX/SynbrAIn srl/AID Patient Summary/1.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://synbrainai-my.sharepoint.com/personal/cristian_zamparini_synbrain_ai/Documents/Desktop/FSE_INTEGRATION/ACCREDITAMENTO/SYNBRAINSRLXX/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://synbrainai-my.sharepoint.com/personal/cristian_zamparini_synbrain_ai/Documents/Desktop/FSE_INTEGRATION/ACCREDITAMENTO/SYNBRAINSRLXX/results_rev1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="210" documentId="11_FFAE48BDFE3911A812E6FAAFDDA9B565C542B408" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74EB2E85-6579-4206-B7EA-2F3BC8D1C56C}"/>
+  <xr:revisionPtr revIDLastSave="321" documentId="11_FFAE48BDFE3911A812E6FAAFDDA9B565C542B408" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AED136BB-EC8A-408B-9FFC-5289347A083B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="531">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -261,15 +261,6 @@
     <t>VALIDAZIONE_TOKEN_JWT_PSS_KO</t>
   </si>
   <si>
-    <t>2026-01-22</t>
-  </si>
-  <si>
-    <t>2026-01-22T17:41:37.665825Z</t>
-  </si>
-  <si>
-    <t>8b39ba65c3126af5634e312a84641731</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -319,12 +310,6 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_PSS_KO</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:38.117853Z</t>
-  </si>
-  <si>
-    <t>c61d6eec302d1a044acc7d0253a87db8</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO</t>
   </si>
   <si>
@@ -1050,15 +1035,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:28.973674Z</t>
-  </si>
-  <si>
-    <t>b728b3fe2d54848bf10fd0bcc27568be</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.b79d4fd451^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT8_KO</t>
   </si>
   <si>
@@ -1066,15 +1042,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:29.443799Z</t>
-  </si>
-  <si>
-    <t>0fa215c2b7040e4fcaba14732ede7a18</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.5ba781cca7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT9_KO</t>
   </si>
   <si>
@@ -1082,15 +1049,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:29.985059Z</t>
-  </si>
-  <si>
-    <t>5e333629274f8d864f74edfbb654b864</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.7d7c60e43e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT10_KO</t>
   </si>
   <si>
@@ -1098,15 +1056,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:30.537769Z</t>
-  </si>
-  <si>
-    <t>dd0947d3cefb3da0717be9ca6422b2e3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.92e7260687^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT11_KO</t>
   </si>
   <si>
@@ -1114,15 +1063,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:31.126298Z</t>
-  </si>
-  <si>
-    <t>4ef582019d899df0fb6dde9998147a09</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.cf9d2f3a51^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT12_KO</t>
   </si>
   <si>
@@ -1130,15 +1070,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:31.637183Z</t>
-  </si>
-  <si>
-    <t>88288a05b9ab589ea5b192df2e377ec7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.daefd57659^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT13_KO</t>
   </si>
   <si>
@@ -1146,15 +1077,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:32.187563Z</t>
-  </si>
-  <si>
-    <t>d2057113a009305ff550f458e40d7a7d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.b4292ed4ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT14_KO</t>
   </si>
   <si>
@@ -1162,15 +1084,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:32.698386Z</t>
-  </si>
-  <si>
-    <t>708d2fbe412ad1427e779a82c0275d3e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.35ccbe662b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT15_KO</t>
   </si>
   <si>
@@ -1178,15 +1091,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:33.297733Z</t>
-  </si>
-  <si>
-    <t>31ddf22fac7aaae5cc023ed3e78e1a9b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.f5bf711743^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT16_KO</t>
   </si>
   <si>
@@ -1194,15 +1098,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:33.857628Z</t>
-  </si>
-  <si>
-    <t>af251b772770ae85e71ddd21454b94f6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.e2bc4ed063^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT17_KO</t>
   </si>
   <si>
@@ -1210,15 +1105,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:34.407233Z</t>
-  </si>
-  <si>
-    <t>5811cd3b27c3de1eed59e1bb69c0fac2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.f7e317af24^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT18_KO</t>
   </si>
   <si>
@@ -1226,15 +1112,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:34.990995Z</t>
-  </si>
-  <si>
-    <t>8043be1e80bc055c0a3fa7fbe7babd28</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.d296a10073^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT19_KO</t>
   </si>
   <si>
@@ -1242,15 +1119,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:35.512475Z</t>
-  </si>
-  <si>
-    <t>eccb5f81fa71091d68007d92cd3f0672</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.aa61a58a23^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT20_KO</t>
   </si>
   <si>
@@ -1258,29 +1126,11 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:36.046474Z</t>
-  </si>
-  <si>
-    <t>f7083e01c6f783661c3e728c3c44467b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.3dc736f1da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT21_KO</t>
   </si>
   <si>
     <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2026-01-22T17:41:36.613348Z</t>
-  </si>
-  <si>
-    <t>ad0c39eaab1fc92bb6a1a1cff573a9bc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.490cc07b9b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_TRASF_CT1</t>
@@ -1556,15 +1406,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:37.135559Z</t>
-  </si>
-  <si>
-    <t>f12ff0dd5c875310a69d611fb157d71a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.bb5aaa6185^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RAP_CT25_KO</t>
   </si>
   <si>
@@ -1615,15 +1456,6 @@
 </t>
   </si>
   <si>
-    <t>2026-01-22T17:41:27.233036Z</t>
-  </si>
-  <si>
-    <t>570ad923626f714fb8a71c6daba6c38f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.76b1f255a4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT24</t>
   </si>
   <si>
@@ -1632,15 +1464,6 @@
 </t>
   </si>
   <si>
-    <t>2026-01-22T17:41:27.801389Z</t>
-  </si>
-  <si>
-    <t>2c77caa7cf5094085f74530c3d4a80f2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.ae2eeab9ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_PSS_CT25</t>
   </si>
   <si>
@@ -1648,15 +1471,6 @@
 Il Documento CDA2 Profilo Sanitario Sintetico dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. Il "CASO DI TEST 25" si riferisce a un esempio di CDA2 semplice, contenente esclusivamente sezioni ed elementi obbligatori previsti dalle specifiche nazionali (IG HL7 Italia)</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:28.406227Z</t>
-  </si>
-  <si>
-    <t>44a027e28fdb67075ca02d5abac6516c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.e39a06b93b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Razionale di Applicabilità</t>
   </si>
   <si>
@@ -1846,15 +1660,199 @@
     <t>Errore in fase di validazione. Controllare i campi obbligatori e reinviare.</t>
   </si>
   <si>
-    <t>2026-01-22T17:41:38.754221Z</t>
+    <t>2026-01-26T18:22:44.948807Z</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:45.906777Z</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:46.354221Z</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:35.044121Z</t>
+  </si>
+  <si>
+    <t>d4683c991725cbc5a99c3baaea1e3d11</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.7ff9835bb4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>7d2d435082106a40a710e26b22e612b1</t>
+  </si>
+  <si>
+    <t>c8b5d2afb8812050e79db749318e793c</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:35.584548Z</t>
+  </si>
+  <si>
+    <t>126ca3942eeb177db629669b24a37428</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.390627db91^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:36.100361Z</t>
+  </si>
+  <si>
+    <t>2e9a99eaff459ad7f58bd5a5fc760509</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.dd7f372da1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:36.622783Z</t>
+  </si>
+  <si>
+    <t>1b0f8465fbe74cd8733222a35a0dd075</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.a6235ea9e9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:37.235281Z</t>
+  </si>
+  <si>
+    <t>58611a18f1eb6adf6986775905de3509</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.132dcde637^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:37.984720Z</t>
+  </si>
+  <si>
+    <t>e6c0992b0e00d369cf6875b5c118416e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.4d469027a8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:38.620098Z</t>
+  </si>
+  <si>
+    <t>ee003e107067e09c7ac0797f25c5067b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.7cd2d4d1c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:39.352449Z</t>
+  </si>
+  <si>
+    <t>ddad2c2f5553c6755b85827181d2d623</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.cbdfee6de9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:40.120266Z</t>
+  </si>
+  <si>
+    <t>4ed709f436904dacba1c3427cadebe13</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.2b471316b8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:40.703841Z</t>
+  </si>
+  <si>
+    <t>a32e263d4342d13d3ca97e93a61b027a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.a466bfaa21^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:41.206489Z</t>
+  </si>
+  <si>
+    <t>bd06c23fede9bc702c88738d8bf3b880</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.e11050379a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:41.774528Z</t>
+  </si>
+  <si>
+    <t>3424228ebf324448ddff85caaf6e1c99</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.e14984d4bc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:42.325171Z</t>
+  </si>
+  <si>
+    <t>9136d7147f47f6470b04e5a0e8f3f042</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.cd49c8aa7f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:42.863989Z</t>
+  </si>
+  <si>
+    <t>693eb36857d6f7515cdde42cf0cb3072</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.c67dc86625^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:43.434398Z</t>
+  </si>
+  <si>
+    <t>dbe7831ff65b3b385be220457ebf1cd7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.4ed6b08040^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:43.990435Z</t>
+  </si>
+  <si>
+    <t>3bdc2a874e093b40c93d481ede00bd95</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.784cbc9076^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:33.084915Z</t>
+  </si>
+  <si>
+    <t>0132cf4ebc362d5de70cdc404fe7546a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.bc0a6bcd37^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4aaea6b38e17f343f9a73cac2cf4ce1d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.a14cf55f59^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:33.811318Z</t>
+  </si>
+  <si>
+    <t>2026-01-26T18:22:34.435139Z</t>
+  </si>
+  <si>
+    <t>c5b412c816103b71efda69345d7e2c48</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.5f8fad5604^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -2293,7 +2291,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2444,6 +2442,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2521,10 +2522,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3895,10 +3892,10 @@
   <dimension ref="A1:W745"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="M13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="I193" sqref="I193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -4312,48 +4309,48 @@
       <c r="E13" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="60">
+        <v>46048</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>469</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="I13" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="I13" s="42" t="s">
-        <v>62</v>
-      </c>
       <c r="J13" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K13" s="38"/>
       <c r="L13" s="38"/>
       <c r="M13" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N13" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O13" s="38" t="s">
-        <v>506</v>
+        <v>444</v>
       </c>
       <c r="P13" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q13" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R13" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S13" s="47" t="s">
-        <v>508</v>
+        <v>446</v>
       </c>
       <c r="T13" s="38"/>
       <c r="U13" s="39"/>
       <c r="V13" s="40" t="s">
-        <v>510</v>
+        <v>448</v>
       </c>
       <c r="W13" s="38" t="s">
         <v>54</v>
@@ -4367,10 +4364,10 @@
         <v>47</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E14" s="43" t="s">
         <v>53</v>
@@ -4404,10 +4401,10 @@
         <v>47</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E15" s="43" t="s">
         <v>53</v>
@@ -4441,10 +4438,10 @@
         <v>47</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E16" s="43" t="s">
         <v>53</v>
@@ -4478,10 +4475,10 @@
         <v>47</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E17" s="43" t="s">
         <v>53</v>
@@ -4515,10 +4512,10 @@
         <v>47</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E18" s="43" t="s">
         <v>53</v>
@@ -4555,10 +4552,10 @@
         <v>48</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F19" s="37"/>
       <c r="G19" s="37"/>
@@ -4592,10 +4589,10 @@
         <v>55</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F20" s="37"/>
       <c r="G20" s="37"/>
@@ -4629,53 +4626,53 @@
         <v>57</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="60">
+        <v>46048</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>470</v>
+      </c>
+      <c r="H21" s="37" t="s">
+        <v>475</v>
+      </c>
+      <c r="I21" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="I21" s="42" t="s">
-        <v>62</v>
-      </c>
       <c r="J21" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K21" s="38"/>
       <c r="L21" s="38"/>
       <c r="M21" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N21" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O21" s="38" t="s">
-        <v>506</v>
+        <v>444</v>
       </c>
       <c r="P21" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q21" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R21" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S21" s="47" t="s">
-        <v>508</v>
+        <v>446</v>
       </c>
       <c r="T21" s="38"/>
       <c r="U21" s="39"/>
       <c r="V21" s="40" t="s">
-        <v>510</v>
+        <v>448</v>
       </c>
       <c r="W21" s="38" t="s">
         <v>54</v>
@@ -4689,13 +4686,13 @@
         <v>47</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F22" s="37"/>
       <c r="G22" s="37"/>
@@ -4726,13 +4723,13 @@
         <v>47</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F23" s="37"/>
       <c r="G23" s="37"/>
@@ -4763,13 +4760,13 @@
         <v>47</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E24" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F24" s="37"/>
       <c r="G24" s="37"/>
@@ -4800,13 +4797,13 @@
         <v>47</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E25" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F25" s="37"/>
       <c r="G25" s="37"/>
@@ -4837,13 +4834,13 @@
         <v>47</v>
       </c>
       <c r="C26" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="43" t="s">
         <v>71</v>
-      </c>
-      <c r="D26" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="43" t="s">
-        <v>74</v>
       </c>
       <c r="F26" s="37"/>
       <c r="G26" s="37"/>
@@ -4877,10 +4874,10 @@
         <v>48</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E27" s="43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
@@ -4898,7 +4895,7 @@
       <c r="S27" s="38"/>
       <c r="T27" s="38"/>
       <c r="U27" s="39" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="V27" s="40"/>
       <c r="W27" s="38" t="s">
@@ -4916,10 +4913,10 @@
         <v>55</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E28" s="43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F28" s="37"/>
       <c r="G28" s="37"/>
@@ -4937,7 +4934,7 @@
       <c r="S28" s="38"/>
       <c r="T28" s="38"/>
       <c r="U28" s="39" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="V28" s="40"/>
       <c r="W28" s="38" t="s">
@@ -4955,48 +4952,48 @@
         <v>57</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E29" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="F29" s="37" t="s">
-        <v>59</v>
+        <v>80</v>
+      </c>
+      <c r="F29" s="60">
+        <v>46048</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>531</v>
+        <v>471</v>
       </c>
       <c r="H29" s="37"/>
       <c r="I29" s="42"/>
       <c r="J29" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K29" s="38"/>
       <c r="L29" s="38"/>
       <c r="M29" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N29" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O29" s="38" t="s">
-        <v>529</v>
+        <v>467</v>
       </c>
       <c r="P29" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q29" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R29" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S29" s="38" t="s">
-        <v>509</v>
+        <v>447</v>
       </c>
       <c r="T29" s="38"/>
       <c r="U29" s="39" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="V29" s="40"/>
       <c r="W29" s="38" t="s">
@@ -5011,13 +5008,13 @@
         <v>47</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
@@ -5035,7 +5032,7 @@
       <c r="S30" s="38"/>
       <c r="T30" s="38"/>
       <c r="U30" s="39" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="V30" s="40"/>
       <c r="W30" s="38" t="s">
@@ -5050,13 +5047,13 @@
         <v>47</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D31" s="35" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E31" s="43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F31" s="37"/>
       <c r="G31" s="37"/>
@@ -5074,7 +5071,7 @@
       <c r="S31" s="38"/>
       <c r="T31" s="38"/>
       <c r="U31" s="39" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="V31" s="40"/>
       <c r="W31" s="38" t="s">
@@ -5089,13 +5086,13 @@
         <v>47</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E32" s="43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F32" s="37"/>
       <c r="G32" s="37"/>
@@ -5113,7 +5110,7 @@
       <c r="S32" s="38"/>
       <c r="T32" s="38"/>
       <c r="U32" s="39" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="V32" s="40"/>
       <c r="W32" s="38" t="s">
@@ -5128,13 +5125,13 @@
         <v>47</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E33" s="43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F33" s="37"/>
       <c r="G33" s="37"/>
@@ -5152,7 +5149,7 @@
       <c r="S33" s="38"/>
       <c r="T33" s="38"/>
       <c r="U33" s="39" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="V33" s="40"/>
       <c r="W33" s="38" t="s">
@@ -5167,13 +5164,13 @@
         <v>47</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F34" s="37"/>
       <c r="G34" s="37"/>
@@ -5191,7 +5188,7 @@
       <c r="S34" s="38"/>
       <c r="T34" s="38"/>
       <c r="U34" s="39" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="V34" s="40"/>
       <c r="W34" s="38" t="s">
@@ -5209,10 +5206,10 @@
         <v>48</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F35" s="37"/>
       <c r="G35" s="37"/>
@@ -5246,10 +5243,10 @@
         <v>48</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
@@ -5283,10 +5280,10 @@
         <v>48</v>
       </c>
       <c r="D37" s="35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F37" s="37"/>
       <c r="G37" s="37"/>
@@ -5320,10 +5317,10 @@
         <v>48</v>
       </c>
       <c r="D38" s="35" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F38" s="37"/>
       <c r="G38" s="37"/>
@@ -5357,10 +5354,10 @@
         <v>48</v>
       </c>
       <c r="D39" s="35" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E39" s="43" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F39" s="37"/>
       <c r="G39" s="37"/>
@@ -5394,10 +5391,10 @@
         <v>48</v>
       </c>
       <c r="D40" s="35" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E40" s="43" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F40" s="37"/>
       <c r="G40" s="37"/>
@@ -5431,10 +5428,10 @@
         <v>48</v>
       </c>
       <c r="D41" s="35" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F41" s="37"/>
       <c r="G41" s="37"/>
@@ -5468,10 +5465,10 @@
         <v>48</v>
       </c>
       <c r="D42" s="35" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E42" s="43" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F42" s="37"/>
       <c r="G42" s="37"/>
@@ -5505,10 +5502,10 @@
         <v>55</v>
       </c>
       <c r="D43" s="35" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E43" s="43" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F43" s="37"/>
       <c r="G43" s="37"/>
@@ -5542,10 +5539,10 @@
         <v>55</v>
       </c>
       <c r="D44" s="35" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E44" s="43" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F44" s="37"/>
       <c r="G44" s="37"/>
@@ -5579,10 +5576,10 @@
         <v>55</v>
       </c>
       <c r="D45" s="35" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E45" s="43" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F45" s="37"/>
       <c r="G45" s="37"/>
@@ -5616,10 +5613,10 @@
         <v>55</v>
       </c>
       <c r="D46" s="35" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E46" s="43" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F46" s="37"/>
       <c r="G46" s="37"/>
@@ -5653,10 +5650,10 @@
         <v>55</v>
       </c>
       <c r="D47" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E47" s="43" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F47" s="37"/>
       <c r="G47" s="37"/>
@@ -5690,10 +5687,10 @@
         <v>55</v>
       </c>
       <c r="D48" s="35" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E48" s="43" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F48" s="37"/>
       <c r="G48" s="37"/>
@@ -5727,10 +5724,10 @@
         <v>55</v>
       </c>
       <c r="D49" s="35" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E49" s="43" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F49" s="37"/>
       <c r="G49" s="37"/>
@@ -5764,10 +5761,10 @@
         <v>55</v>
       </c>
       <c r="D50" s="35" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E50" s="43" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F50" s="37"/>
       <c r="G50" s="37"/>
@@ -5801,10 +5798,10 @@
         <v>55</v>
       </c>
       <c r="D51" s="35" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F51" s="37"/>
       <c r="G51" s="37"/>
@@ -5838,10 +5835,10 @@
         <v>55</v>
       </c>
       <c r="D52" s="35" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E52" s="43" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F52" s="37"/>
       <c r="G52" s="37"/>
@@ -5872,13 +5869,13 @@
         <v>47</v>
       </c>
       <c r="C53" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D53" s="35" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F53" s="37"/>
       <c r="G53" s="37"/>
@@ -5909,13 +5906,13 @@
         <v>47</v>
       </c>
       <c r="C54" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D54" s="35" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E54" s="43" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F54" s="37"/>
       <c r="G54" s="37"/>
@@ -5946,13 +5943,13 @@
         <v>47</v>
       </c>
       <c r="C55" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D55" s="35" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E55" s="43" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F55" s="37"/>
       <c r="G55" s="37"/>
@@ -5983,13 +5980,13 @@
         <v>47</v>
       </c>
       <c r="C56" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D56" s="35" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F56" s="37"/>
       <c r="G56" s="37"/>
@@ -6020,13 +6017,13 @@
         <v>47</v>
       </c>
       <c r="C57" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D57" s="35" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F57" s="37"/>
       <c r="G57" s="37"/>
@@ -6057,13 +6054,13 @@
         <v>47</v>
       </c>
       <c r="C58" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D58" s="35" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E58" s="43" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F58" s="37"/>
       <c r="G58" s="37"/>
@@ -6094,13 +6091,13 @@
         <v>47</v>
       </c>
       <c r="C59" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D59" s="35" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E59" s="43" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F59" s="37"/>
       <c r="G59" s="37"/>
@@ -6131,13 +6128,13 @@
         <v>47</v>
       </c>
       <c r="C60" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D60" s="35" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E60" s="43" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F60" s="37"/>
       <c r="G60" s="37"/>
@@ -6168,13 +6165,13 @@
         <v>47</v>
       </c>
       <c r="C61" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D61" s="35" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E61" s="43" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F61" s="37"/>
       <c r="G61" s="37"/>
@@ -6205,13 +6202,13 @@
         <v>47</v>
       </c>
       <c r="C62" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D62" s="35" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E62" s="43" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F62" s="37"/>
       <c r="G62" s="37"/>
@@ -6242,13 +6239,13 @@
         <v>47</v>
       </c>
       <c r="C63" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D63" s="35" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F63" s="37"/>
       <c r="G63" s="37"/>
@@ -6279,13 +6276,13 @@
         <v>47</v>
       </c>
       <c r="C64" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D64" s="35" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E64" s="43" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F64" s="37"/>
       <c r="G64" s="37"/>
@@ -6316,13 +6313,13 @@
         <v>47</v>
       </c>
       <c r="C65" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D65" s="35" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E65" s="43" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F65" s="37"/>
       <c r="G65" s="37"/>
@@ -6353,13 +6350,13 @@
         <v>47</v>
       </c>
       <c r="C66" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D66" s="35" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E66" s="43" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F66" s="37"/>
       <c r="G66" s="37"/>
@@ -6390,13 +6387,13 @@
         <v>47</v>
       </c>
       <c r="C67" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E67" s="43" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
@@ -6427,13 +6424,13 @@
         <v>47</v>
       </c>
       <c r="C68" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D68" s="35" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E68" s="43" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F68" s="37"/>
       <c r="G68" s="37"/>
@@ -6464,13 +6461,13 @@
         <v>47</v>
       </c>
       <c r="C69" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D69" s="35" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E69" s="43" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F69" s="37"/>
       <c r="G69" s="37"/>
@@ -6501,13 +6498,13 @@
         <v>47</v>
       </c>
       <c r="C70" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D70" s="35" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E70" s="43" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F70" s="37"/>
       <c r="G70" s="37"/>
@@ -6538,13 +6535,13 @@
         <v>47</v>
       </c>
       <c r="C71" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D71" s="35" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E71" s="43" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F71" s="37"/>
       <c r="G71" s="37"/>
@@ -6575,13 +6572,13 @@
         <v>47</v>
       </c>
       <c r="C72" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D72" s="35" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E72" s="43" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F72" s="37"/>
       <c r="G72" s="37"/>
@@ -6612,13 +6609,13 @@
         <v>47</v>
       </c>
       <c r="C73" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D73" s="35" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E73" s="43" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F73" s="37"/>
       <c r="G73" s="37"/>
@@ -6649,13 +6646,13 @@
         <v>47</v>
       </c>
       <c r="C74" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D74" s="35" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E74" s="43" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F74" s="37"/>
       <c r="G74" s="37"/>
@@ -6686,13 +6683,13 @@
         <v>47</v>
       </c>
       <c r="C75" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D75" s="35" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E75" s="43" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F75" s="37"/>
       <c r="G75" s="37"/>
@@ -6723,13 +6720,13 @@
         <v>47</v>
       </c>
       <c r="C76" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D76" s="35" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E76" s="43" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F76" s="37"/>
       <c r="G76" s="37"/>
@@ -6760,13 +6757,13 @@
         <v>47</v>
       </c>
       <c r="C77" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D77" s="35" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E77" s="43" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F77" s="37"/>
       <c r="G77" s="37"/>
@@ -6797,13 +6794,13 @@
         <v>47</v>
       </c>
       <c r="C78" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D78" s="35" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E78" s="43" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F78" s="37"/>
       <c r="G78" s="37"/>
@@ -6834,13 +6831,13 @@
         <v>47</v>
       </c>
       <c r="C79" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D79" s="35" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E79" s="43" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F79" s="37"/>
       <c r="G79" s="37"/>
@@ -6871,13 +6868,13 @@
         <v>47</v>
       </c>
       <c r="C80" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D80" s="35" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E80" s="43" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F80" s="37"/>
       <c r="G80" s="37"/>
@@ -6908,13 +6905,13 @@
         <v>47</v>
       </c>
       <c r="C81" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D81" s="35" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E81" s="43" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F81" s="37"/>
       <c r="G81" s="37"/>
@@ -6945,13 +6942,13 @@
         <v>47</v>
       </c>
       <c r="C82" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D82" s="35" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E82" s="43" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F82" s="37"/>
       <c r="G82" s="37"/>
@@ -6982,13 +6979,13 @@
         <v>47</v>
       </c>
       <c r="C83" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D83" s="35" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E83" s="43" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F83" s="37"/>
       <c r="G83" s="37"/>
@@ -7019,13 +7016,13 @@
         <v>47</v>
       </c>
       <c r="C84" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D84" s="35" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E84" s="43" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F84" s="37"/>
       <c r="G84" s="37"/>
@@ -7056,13 +7053,13 @@
         <v>47</v>
       </c>
       <c r="C85" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D85" s="35" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E85" s="43" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F85" s="37"/>
       <c r="G85" s="37"/>
@@ -7093,13 +7090,13 @@
         <v>47</v>
       </c>
       <c r="C86" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D86" s="35" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E86" s="43" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F86" s="37"/>
       <c r="G86" s="37"/>
@@ -7130,13 +7127,13 @@
         <v>47</v>
       </c>
       <c r="C87" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D87" s="35" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E87" s="43" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F87" s="37"/>
       <c r="G87" s="37"/>
@@ -7167,13 +7164,13 @@
         <v>47</v>
       </c>
       <c r="C88" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D88" s="35" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E88" s="43" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F88" s="37"/>
       <c r="G88" s="37"/>
@@ -7204,13 +7201,13 @@
         <v>47</v>
       </c>
       <c r="C89" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D89" s="35" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E89" s="43" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F89" s="37"/>
       <c r="G89" s="37"/>
@@ -7241,13 +7238,13 @@
         <v>47</v>
       </c>
       <c r="C90" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D90" s="35" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E90" s="43" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F90" s="37"/>
       <c r="G90" s="37"/>
@@ -7278,13 +7275,13 @@
         <v>47</v>
       </c>
       <c r="C91" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D91" s="35" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E91" s="43" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F91" s="37"/>
       <c r="G91" s="37"/>
@@ -7315,13 +7312,13 @@
         <v>47</v>
       </c>
       <c r="C92" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D92" s="35" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E92" s="43" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F92" s="37"/>
       <c r="G92" s="37"/>
@@ -7352,13 +7349,13 @@
         <v>47</v>
       </c>
       <c r="C93" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D93" s="35" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E93" s="43" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F93" s="37"/>
       <c r="G93" s="37"/>
@@ -7389,13 +7386,13 @@
         <v>47</v>
       </c>
       <c r="C94" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D94" s="35" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E94" s="43" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F94" s="37"/>
       <c r="G94" s="37"/>
@@ -7426,13 +7423,13 @@
         <v>47</v>
       </c>
       <c r="C95" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D95" s="35" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E95" s="43" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F95" s="37"/>
       <c r="G95" s="37"/>
@@ -7463,13 +7460,13 @@
         <v>47</v>
       </c>
       <c r="C96" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D96" s="35" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E96" s="43" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F96" s="37"/>
       <c r="G96" s="37"/>
@@ -7500,13 +7497,13 @@
         <v>47</v>
       </c>
       <c r="C97" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D97" s="35" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E97" s="43" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F97" s="37"/>
       <c r="G97" s="37"/>
@@ -7537,13 +7534,13 @@
         <v>47</v>
       </c>
       <c r="C98" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D98" s="35" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E98" s="43" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F98" s="37"/>
       <c r="G98" s="37"/>
@@ -7574,13 +7571,13 @@
         <v>47</v>
       </c>
       <c r="C99" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D99" s="35" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E99" s="43" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F99" s="37"/>
       <c r="G99" s="37"/>
@@ -7611,13 +7608,13 @@
         <v>47</v>
       </c>
       <c r="C100" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D100" s="35" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E100" s="43" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F100" s="37"/>
       <c r="G100" s="37"/>
@@ -7648,13 +7645,13 @@
         <v>47</v>
       </c>
       <c r="C101" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D101" s="35" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F101" s="37"/>
       <c r="G101" s="37"/>
@@ -7685,13 +7682,13 @@
         <v>47</v>
       </c>
       <c r="C102" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D102" s="35" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E102" s="43" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F102" s="37"/>
       <c r="G102" s="37"/>
@@ -7722,13 +7719,13 @@
         <v>47</v>
       </c>
       <c r="C103" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D103" s="35" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E103" s="43" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F103" s="37"/>
       <c r="G103" s="37"/>
@@ -7759,13 +7756,13 @@
         <v>47</v>
       </c>
       <c r="C104" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D104" s="35" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E104" s="43" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F104" s="37"/>
       <c r="G104" s="37"/>
@@ -7796,13 +7793,13 @@
         <v>47</v>
       </c>
       <c r="C105" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D105" s="35" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E105" s="43" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F105" s="37"/>
       <c r="G105" s="37"/>
@@ -7833,13 +7830,13 @@
         <v>47</v>
       </c>
       <c r="C106" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D106" s="35" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E106" s="43" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F106" s="37"/>
       <c r="G106" s="37"/>
@@ -7870,13 +7867,13 @@
         <v>47</v>
       </c>
       <c r="C107" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D107" s="35" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E107" s="43" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F107" s="37"/>
       <c r="G107" s="37"/>
@@ -7907,13 +7904,13 @@
         <v>47</v>
       </c>
       <c r="C108" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D108" s="35" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E108" s="43" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F108" s="37"/>
       <c r="G108" s="37"/>
@@ -7944,13 +7941,13 @@
         <v>47</v>
       </c>
       <c r="C109" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D109" s="35" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E109" s="43" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F109" s="37"/>
       <c r="G109" s="37"/>
@@ -7981,13 +7978,13 @@
         <v>47</v>
       </c>
       <c r="C110" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D110" s="35" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E110" s="43" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="F110" s="37"/>
       <c r="G110" s="37"/>
@@ -8018,13 +8015,13 @@
         <v>47</v>
       </c>
       <c r="C111" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D111" s="35" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E111" s="43" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F111" s="37"/>
       <c r="G111" s="37"/>
@@ -8055,13 +8052,13 @@
         <v>47</v>
       </c>
       <c r="C112" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D112" s="35" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E112" s="43" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F112" s="37"/>
       <c r="G112" s="37"/>
@@ -8092,13 +8089,13 @@
         <v>47</v>
       </c>
       <c r="C113" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D113" s="35" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E113" s="43" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F113" s="37"/>
       <c r="G113" s="37"/>
@@ -8129,13 +8126,13 @@
         <v>47</v>
       </c>
       <c r="C114" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D114" s="35" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E114" s="43" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F114" s="37"/>
       <c r="G114" s="37"/>
@@ -8166,13 +8163,13 @@
         <v>47</v>
       </c>
       <c r="C115" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D115" s="35" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E115" s="43" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F115" s="37"/>
       <c r="G115" s="37"/>
@@ -8203,13 +8200,13 @@
         <v>47</v>
       </c>
       <c r="C116" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D116" s="35" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E116" s="43" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F116" s="37"/>
       <c r="G116" s="37"/>
@@ -8240,13 +8237,13 @@
         <v>47</v>
       </c>
       <c r="C117" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D117" s="35" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E117" s="43" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F117" s="37"/>
       <c r="G117" s="37"/>
@@ -8277,13 +8274,13 @@
         <v>47</v>
       </c>
       <c r="C118" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D118" s="35" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E118" s="43" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F118" s="37"/>
       <c r="G118" s="37"/>
@@ -8314,13 +8311,13 @@
         <v>47</v>
       </c>
       <c r="C119" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D119" s="35" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="E119" s="43" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="F119" s="37"/>
       <c r="G119" s="37"/>
@@ -8351,13 +8348,13 @@
         <v>47</v>
       </c>
       <c r="C120" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D120" s="35" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E120" s="43" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F120" s="37"/>
       <c r="G120" s="37"/>
@@ -8388,13 +8385,13 @@
         <v>47</v>
       </c>
       <c r="C121" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D121" s="35" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E121" s="43" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F121" s="37"/>
       <c r="G121" s="37"/>
@@ -8425,13 +8422,13 @@
         <v>47</v>
       </c>
       <c r="C122" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D122" s="35" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E122" s="43" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="F122" s="37"/>
       <c r="G122" s="37"/>
@@ -8462,13 +8459,13 @@
         <v>47</v>
       </c>
       <c r="C123" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D123" s="35" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E123" s="43" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F123" s="37"/>
       <c r="G123" s="37"/>
@@ -8499,13 +8496,13 @@
         <v>47</v>
       </c>
       <c r="C124" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D124" s="35" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E124" s="43" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F124" s="37"/>
       <c r="G124" s="37"/>
@@ -8536,13 +8533,13 @@
         <v>47</v>
       </c>
       <c r="C125" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D125" s="35" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E125" s="43" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F125" s="37"/>
       <c r="G125" s="37"/>
@@ -8573,13 +8570,13 @@
         <v>47</v>
       </c>
       <c r="C126" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D126" s="35" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E126" s="43" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F126" s="37"/>
       <c r="G126" s="37"/>
@@ -8610,13 +8607,13 @@
         <v>47</v>
       </c>
       <c r="C127" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D127" s="35" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E127" s="43" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="F127" s="37"/>
       <c r="G127" s="37"/>
@@ -8647,13 +8644,13 @@
         <v>47</v>
       </c>
       <c r="C128" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D128" s="35" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E128" s="43" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F128" s="37"/>
       <c r="G128" s="37"/>
@@ -8684,13 +8681,13 @@
         <v>47</v>
       </c>
       <c r="C129" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D129" s="35" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E129" s="43" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F129" s="37"/>
       <c r="G129" s="37"/>
@@ -8721,13 +8718,13 @@
         <v>47</v>
       </c>
       <c r="C130" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D130" s="35" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E130" s="43" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="F130" s="37"/>
       <c r="G130" s="37"/>
@@ -8761,53 +8758,53 @@
         <v>57</v>
       </c>
       <c r="D131" s="35" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="E131" s="43" t="s">
-        <v>287</v>
-      </c>
-      <c r="F131" s="37" t="s">
-        <v>59</v>
+        <v>282</v>
+      </c>
+      <c r="F131" s="60">
+        <v>46048</v>
       </c>
       <c r="G131" s="37" t="s">
-        <v>288</v>
+        <v>472</v>
       </c>
       <c r="H131" s="37" t="s">
-        <v>289</v>
+        <v>473</v>
       </c>
       <c r="I131" s="42" t="s">
-        <v>290</v>
+        <v>474</v>
       </c>
       <c r="J131" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K131" s="38"/>
       <c r="L131" s="38"/>
       <c r="M131" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N131" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O131" s="38" t="s">
-        <v>506</v>
+        <v>444</v>
       </c>
       <c r="P131" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q131" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R131" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S131" s="47" t="s">
-        <v>508</v>
+        <v>446</v>
       </c>
       <c r="T131" s="35"/>
       <c r="U131" s="39"/>
       <c r="V131" s="40" t="s">
-        <v>511</v>
+        <v>449</v>
       </c>
       <c r="W131" s="38" t="s">
         <v>54</v>
@@ -8824,53 +8821,53 @@
         <v>57</v>
       </c>
       <c r="D132" s="35" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E132" s="43" t="s">
-        <v>292</v>
-      </c>
-      <c r="F132" s="37" t="s">
-        <v>59</v>
+        <v>284</v>
+      </c>
+      <c r="F132" s="60">
+        <v>46048</v>
       </c>
       <c r="G132" s="37" t="s">
-        <v>293</v>
+        <v>477</v>
       </c>
       <c r="H132" s="37" t="s">
-        <v>294</v>
+        <v>478</v>
       </c>
       <c r="I132" s="42" t="s">
-        <v>295</v>
+        <v>479</v>
       </c>
       <c r="J132" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K132" s="38"/>
       <c r="L132" s="38"/>
       <c r="M132" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N132" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O132" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P132" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q132" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R132" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S132" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T132" s="35"/>
       <c r="U132" s="39"/>
       <c r="V132" s="40" t="s">
-        <v>512</v>
+        <v>450</v>
       </c>
       <c r="W132" s="38" t="s">
         <v>54</v>
@@ -8887,53 +8884,53 @@
         <v>57</v>
       </c>
       <c r="D133" s="35" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="E133" s="43" t="s">
-        <v>297</v>
-      </c>
-      <c r="F133" s="37" t="s">
-        <v>59</v>
+        <v>286</v>
+      </c>
+      <c r="F133" s="60">
+        <v>46048</v>
       </c>
       <c r="G133" s="37" t="s">
-        <v>298</v>
+        <v>480</v>
       </c>
       <c r="H133" s="37" t="s">
-        <v>299</v>
+        <v>481</v>
       </c>
       <c r="I133" s="42" t="s">
-        <v>300</v>
+        <v>482</v>
       </c>
       <c r="J133" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K133" s="38"/>
       <c r="L133" s="38"/>
       <c r="M133" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N133" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O133" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P133" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q133" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R133" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S133" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T133" s="35"/>
       <c r="U133" s="39"/>
       <c r="V133" s="40" t="s">
-        <v>513</v>
+        <v>451</v>
       </c>
       <c r="W133" s="38" t="s">
         <v>54</v>
@@ -8950,53 +8947,53 @@
         <v>57</v>
       </c>
       <c r="D134" s="35" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="E134" s="43" t="s">
-        <v>302</v>
-      </c>
-      <c r="F134" s="37" t="s">
-        <v>59</v>
+        <v>288</v>
+      </c>
+      <c r="F134" s="60">
+        <v>46048</v>
       </c>
       <c r="G134" s="37" t="s">
-        <v>303</v>
+        <v>483</v>
       </c>
       <c r="H134" s="37" t="s">
-        <v>304</v>
+        <v>484</v>
       </c>
       <c r="I134" s="42" t="s">
-        <v>305</v>
+        <v>485</v>
       </c>
       <c r="J134" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K134" s="38"/>
       <c r="L134" s="38"/>
       <c r="M134" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N134" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O134" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P134" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q134" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R134" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S134" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T134" s="35"/>
       <c r="U134" s="39"/>
       <c r="V134" s="40" t="s">
-        <v>514</v>
+        <v>452</v>
       </c>
       <c r="W134" s="38" t="s">
         <v>54</v>
@@ -9013,53 +9010,53 @@
         <v>57</v>
       </c>
       <c r="D135" s="35" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="E135" s="43" t="s">
-        <v>307</v>
-      </c>
-      <c r="F135" s="37" t="s">
-        <v>59</v>
+        <v>290</v>
+      </c>
+      <c r="F135" s="60">
+        <v>46048</v>
       </c>
       <c r="G135" s="37" t="s">
-        <v>308</v>
+        <v>486</v>
       </c>
       <c r="H135" s="37" t="s">
-        <v>309</v>
+        <v>487</v>
       </c>
       <c r="I135" s="42" t="s">
-        <v>310</v>
+        <v>488</v>
       </c>
       <c r="J135" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K135" s="38"/>
       <c r="L135" s="38"/>
       <c r="M135" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N135" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O135" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P135" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q135" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R135" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S135" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T135" s="35"/>
       <c r="U135" s="39"/>
       <c r="V135" s="40" t="s">
-        <v>515</v>
+        <v>453</v>
       </c>
       <c r="W135" s="38" t="s">
         <v>54</v>
@@ -9076,53 +9073,53 @@
         <v>57</v>
       </c>
       <c r="D136" s="35" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="E136" s="43" t="s">
-        <v>312</v>
-      </c>
-      <c r="F136" s="37" t="s">
-        <v>59</v>
+        <v>292</v>
+      </c>
+      <c r="F136" s="60">
+        <v>46048</v>
       </c>
       <c r="G136" s="37" t="s">
-        <v>313</v>
+        <v>489</v>
       </c>
       <c r="H136" s="37" t="s">
-        <v>314</v>
+        <v>490</v>
       </c>
       <c r="I136" s="42" t="s">
-        <v>315</v>
+        <v>491</v>
       </c>
       <c r="J136" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K136" s="38"/>
       <c r="L136" s="38"/>
       <c r="M136" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N136" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O136" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P136" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q136" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R136" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S136" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T136" s="35"/>
       <c r="U136" s="39"/>
       <c r="V136" s="40" t="s">
-        <v>516</v>
+        <v>454</v>
       </c>
       <c r="W136" s="38" t="s">
         <v>54</v>
@@ -9139,53 +9136,53 @@
         <v>57</v>
       </c>
       <c r="D137" s="35" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="E137" s="43" t="s">
-        <v>317</v>
-      </c>
-      <c r="F137" s="37" t="s">
-        <v>59</v>
+        <v>294</v>
+      </c>
+      <c r="F137" s="60">
+        <v>46048</v>
       </c>
       <c r="G137" s="37" t="s">
-        <v>318</v>
+        <v>492</v>
       </c>
       <c r="H137" s="37" t="s">
-        <v>319</v>
+        <v>493</v>
       </c>
       <c r="I137" s="42" t="s">
-        <v>320</v>
+        <v>494</v>
       </c>
       <c r="J137" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K137" s="38"/>
       <c r="L137" s="38"/>
       <c r="M137" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N137" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O137" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P137" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q137" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R137" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S137" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T137" s="35"/>
       <c r="U137" s="39"/>
       <c r="V137" s="40" t="s">
-        <v>517</v>
+        <v>455</v>
       </c>
       <c r="W137" s="38" t="s">
         <v>54</v>
@@ -9202,53 +9199,53 @@
         <v>57</v>
       </c>
       <c r="D138" s="35" t="s">
-        <v>321</v>
+        <v>295</v>
       </c>
       <c r="E138" s="43" t="s">
-        <v>322</v>
-      </c>
-      <c r="F138" s="37" t="s">
-        <v>59</v>
+        <v>296</v>
+      </c>
+      <c r="F138" s="60">
+        <v>46048</v>
       </c>
       <c r="G138" s="37" t="s">
-        <v>323</v>
+        <v>495</v>
       </c>
       <c r="H138" s="37" t="s">
-        <v>324</v>
+        <v>496</v>
       </c>
       <c r="I138" s="42" t="s">
-        <v>325</v>
+        <v>497</v>
       </c>
       <c r="J138" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K138" s="38"/>
       <c r="L138" s="38"/>
       <c r="M138" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N138" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O138" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P138" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q138" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R138" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S138" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T138" s="35"/>
       <c r="U138" s="39"/>
       <c r="V138" s="40" t="s">
-        <v>518</v>
+        <v>456</v>
       </c>
       <c r="W138" s="38" t="s">
         <v>54</v>
@@ -9265,53 +9262,53 @@
         <v>57</v>
       </c>
       <c r="D139" s="35" t="s">
-        <v>326</v>
+        <v>297</v>
       </c>
       <c r="E139" s="43" t="s">
-        <v>327</v>
-      </c>
-      <c r="F139" s="37" t="s">
-        <v>59</v>
+        <v>298</v>
+      </c>
+      <c r="F139" s="60">
+        <v>46048</v>
       </c>
       <c r="G139" s="37" t="s">
-        <v>328</v>
+        <v>498</v>
       </c>
       <c r="H139" s="37" t="s">
-        <v>329</v>
+        <v>499</v>
       </c>
       <c r="I139" s="42" t="s">
-        <v>330</v>
+        <v>500</v>
       </c>
       <c r="J139" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K139" s="38"/>
       <c r="L139" s="38"/>
       <c r="M139" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N139" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O139" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P139" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q139" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R139" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S139" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T139" s="35"/>
       <c r="U139" s="39"/>
       <c r="V139" s="40" t="s">
-        <v>519</v>
+        <v>457</v>
       </c>
       <c r="W139" s="38" t="s">
         <v>54</v>
@@ -9328,53 +9325,53 @@
         <v>57</v>
       </c>
       <c r="D140" s="35" t="s">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="E140" s="43" t="s">
-        <v>332</v>
-      </c>
-      <c r="F140" s="37" t="s">
-        <v>59</v>
+        <v>300</v>
+      </c>
+      <c r="F140" s="60">
+        <v>46048</v>
       </c>
       <c r="G140" s="37" t="s">
-        <v>333</v>
+        <v>501</v>
       </c>
       <c r="H140" s="37" t="s">
-        <v>334</v>
+        <v>502</v>
       </c>
       <c r="I140" s="42" t="s">
-        <v>335</v>
+        <v>503</v>
       </c>
       <c r="J140" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K140" s="38"/>
       <c r="L140" s="38"/>
       <c r="M140" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N140" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O140" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P140" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q140" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R140" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S140" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T140" s="35"/>
       <c r="U140" s="39"/>
       <c r="V140" s="40" t="s">
-        <v>520</v>
+        <v>458</v>
       </c>
       <c r="W140" s="38" t="s">
         <v>54</v>
@@ -9391,53 +9388,53 @@
         <v>57</v>
       </c>
       <c r="D141" s="35" t="s">
-        <v>336</v>
+        <v>301</v>
       </c>
       <c r="E141" s="43" t="s">
-        <v>337</v>
-      </c>
-      <c r="F141" s="37" t="s">
-        <v>59</v>
+        <v>302</v>
+      </c>
+      <c r="F141" s="60">
+        <v>46048</v>
       </c>
       <c r="G141" s="37" t="s">
-        <v>338</v>
+        <v>504</v>
       </c>
       <c r="H141" s="37" t="s">
-        <v>339</v>
+        <v>505</v>
       </c>
       <c r="I141" s="42" t="s">
-        <v>340</v>
+        <v>506</v>
       </c>
       <c r="J141" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K141" s="38"/>
       <c r="L141" s="38"/>
       <c r="M141" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N141" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O141" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P141" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q141" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R141" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S141" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T141" s="35"/>
       <c r="U141" s="39"/>
       <c r="V141" s="40" t="s">
-        <v>521</v>
+        <v>459</v>
       </c>
       <c r="W141" s="38" t="s">
         <v>54</v>
@@ -9454,53 +9451,53 @@
         <v>57</v>
       </c>
       <c r="D142" s="35" t="s">
-        <v>341</v>
+        <v>303</v>
       </c>
       <c r="E142" s="43" t="s">
-        <v>342</v>
-      </c>
-      <c r="F142" s="37" t="s">
-        <v>59</v>
+        <v>304</v>
+      </c>
+      <c r="F142" s="60">
+        <v>46048</v>
       </c>
       <c r="G142" s="37" t="s">
-        <v>343</v>
+        <v>507</v>
       </c>
       <c r="H142" s="37" t="s">
-        <v>344</v>
+        <v>508</v>
       </c>
       <c r="I142" s="42" t="s">
-        <v>345</v>
+        <v>509</v>
       </c>
       <c r="J142" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K142" s="38"/>
       <c r="L142" s="38"/>
       <c r="M142" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N142" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O142" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P142" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q142" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R142" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S142" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T142" s="35"/>
       <c r="U142" s="39"/>
       <c r="V142" s="40" t="s">
-        <v>522</v>
+        <v>460</v>
       </c>
       <c r="W142" s="38" t="s">
         <v>54</v>
@@ -9517,53 +9514,53 @@
         <v>57</v>
       </c>
       <c r="D143" s="35" t="s">
-        <v>346</v>
+        <v>305</v>
       </c>
       <c r="E143" s="43" t="s">
-        <v>347</v>
-      </c>
-      <c r="F143" s="37" t="s">
-        <v>59</v>
+        <v>306</v>
+      </c>
+      <c r="F143" s="60">
+        <v>46048</v>
       </c>
       <c r="G143" s="37" t="s">
-        <v>348</v>
+        <v>510</v>
       </c>
       <c r="H143" s="37" t="s">
-        <v>349</v>
+        <v>511</v>
       </c>
       <c r="I143" s="42" t="s">
-        <v>350</v>
+        <v>512</v>
       </c>
       <c r="J143" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K143" s="38"/>
       <c r="L143" s="38"/>
       <c r="M143" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N143" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O143" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P143" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q143" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R143" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S143" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T143" s="35"/>
       <c r="U143" s="39"/>
       <c r="V143" s="40" t="s">
-        <v>523</v>
+        <v>461</v>
       </c>
       <c r="W143" s="38" t="s">
         <v>54</v>
@@ -9580,53 +9577,53 @@
         <v>57</v>
       </c>
       <c r="D144" s="35" t="s">
-        <v>351</v>
+        <v>307</v>
       </c>
       <c r="E144" s="43" t="s">
-        <v>352</v>
-      </c>
-      <c r="F144" s="37" t="s">
-        <v>59</v>
+        <v>308</v>
+      </c>
+      <c r="F144" s="60">
+        <v>46048</v>
       </c>
       <c r="G144" s="37" t="s">
-        <v>353</v>
+        <v>513</v>
       </c>
       <c r="H144" s="37" t="s">
-        <v>354</v>
+        <v>514</v>
       </c>
       <c r="I144" s="42" t="s">
-        <v>355</v>
+        <v>515</v>
       </c>
       <c r="J144" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K144" s="38"/>
       <c r="L144" s="38"/>
       <c r="M144" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N144" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O144" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P144" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q144" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R144" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S144" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T144" s="35"/>
       <c r="U144" s="39"/>
       <c r="V144" s="40" t="s">
-        <v>524</v>
+        <v>462</v>
       </c>
       <c r="W144" s="38" t="s">
         <v>54</v>
@@ -9643,53 +9640,53 @@
         <v>57</v>
       </c>
       <c r="D145" s="35" t="s">
-        <v>356</v>
+        <v>309</v>
       </c>
       <c r="E145" s="43" t="s">
-        <v>357</v>
-      </c>
-      <c r="F145" s="37" t="s">
-        <v>59</v>
+        <v>310</v>
+      </c>
+      <c r="F145" s="60">
+        <v>46048</v>
       </c>
       <c r="G145" s="37" t="s">
-        <v>358</v>
+        <v>516</v>
       </c>
       <c r="H145" s="37" t="s">
-        <v>359</v>
+        <v>517</v>
       </c>
       <c r="I145" s="42" t="s">
-        <v>360</v>
+        <v>518</v>
       </c>
       <c r="J145" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K145" s="38"/>
       <c r="L145" s="38"/>
       <c r="M145" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N145" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O145" s="38" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P145" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q145" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R145" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S145" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T145" s="35"/>
       <c r="U145" s="39"/>
       <c r="V145" s="40" t="s">
-        <v>525</v>
+        <v>463</v>
       </c>
       <c r="W145" s="38" t="s">
         <v>54</v>
@@ -9706,10 +9703,10 @@
         <v>48</v>
       </c>
       <c r="D146" s="35" t="s">
-        <v>361</v>
+        <v>311</v>
       </c>
       <c r="E146" s="43" t="s">
-        <v>362</v>
+        <v>312</v>
       </c>
       <c r="F146" s="37"/>
       <c r="G146" s="37"/>
@@ -9743,10 +9740,10 @@
         <v>48</v>
       </c>
       <c r="D147" s="35" t="s">
-        <v>363</v>
+        <v>313</v>
       </c>
       <c r="E147" s="43" t="s">
-        <v>364</v>
+        <v>314</v>
       </c>
       <c r="F147" s="37"/>
       <c r="G147" s="37"/>
@@ -9777,13 +9774,13 @@
         <v>47</v>
       </c>
       <c r="C148" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D148" s="35" t="s">
-        <v>366</v>
+        <v>316</v>
       </c>
       <c r="E148" s="43" t="s">
-        <v>367</v>
+        <v>317</v>
       </c>
       <c r="F148" s="37"/>
       <c r="G148" s="37"/>
@@ -9814,13 +9811,13 @@
         <v>47</v>
       </c>
       <c r="C149" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D149" s="35" t="s">
-        <v>368</v>
+        <v>318</v>
       </c>
       <c r="E149" s="43" t="s">
-        <v>369</v>
+        <v>319</v>
       </c>
       <c r="F149" s="37"/>
       <c r="G149" s="37"/>
@@ -9851,13 +9848,13 @@
         <v>47</v>
       </c>
       <c r="C150" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D150" s="35" t="s">
-        <v>370</v>
+        <v>320</v>
       </c>
       <c r="E150" s="43" t="s">
-        <v>371</v>
+        <v>321</v>
       </c>
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
@@ -9888,10 +9885,10 @@
         <v>47</v>
       </c>
       <c r="C151" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D151" s="35" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="E151" s="43" t="s">
         <v>53</v>
@@ -9925,13 +9922,13 @@
         <v>47</v>
       </c>
       <c r="C152" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D152" s="35" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="E152" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F152" s="37"/>
       <c r="G152" s="37"/>
@@ -9962,13 +9959,13 @@
         <v>47</v>
       </c>
       <c r="C153" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D153" s="35" t="s">
-        <v>374</v>
+        <v>324</v>
       </c>
       <c r="E153" s="43" t="s">
-        <v>375</v>
+        <v>325</v>
       </c>
       <c r="F153" s="37"/>
       <c r="G153" s="37"/>
@@ -9999,13 +9996,13 @@
         <v>47</v>
       </c>
       <c r="C154" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D154" s="35" t="s">
-        <v>376</v>
+        <v>326</v>
       </c>
       <c r="E154" s="43" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
       <c r="F154" s="37"/>
       <c r="G154" s="37"/>
@@ -10036,13 +10033,13 @@
         <v>47</v>
       </c>
       <c r="C155" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D155" s="35" t="s">
-        <v>378</v>
+        <v>328</v>
       </c>
       <c r="E155" s="43" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
       <c r="F155" s="37"/>
       <c r="G155" s="37"/>
@@ -10073,13 +10070,13 @@
         <v>47</v>
       </c>
       <c r="C156" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D156" s="35" t="s">
-        <v>380</v>
+        <v>330</v>
       </c>
       <c r="E156" s="43" t="s">
-        <v>381</v>
+        <v>331</v>
       </c>
       <c r="F156" s="37"/>
       <c r="G156" s="37"/>
@@ -10110,13 +10107,13 @@
         <v>47</v>
       </c>
       <c r="C157" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D157" s="35" t="s">
-        <v>382</v>
+        <v>332</v>
       </c>
       <c r="E157" s="43" t="s">
-        <v>383</v>
+        <v>333</v>
       </c>
       <c r="F157" s="37"/>
       <c r="G157" s="37"/>
@@ -10147,13 +10144,13 @@
         <v>47</v>
       </c>
       <c r="C158" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D158" s="35" t="s">
-        <v>384</v>
+        <v>334</v>
       </c>
       <c r="E158" s="43" t="s">
-        <v>385</v>
+        <v>335</v>
       </c>
       <c r="F158" s="37"/>
       <c r="G158" s="37"/>
@@ -10184,13 +10181,13 @@
         <v>47</v>
       </c>
       <c r="C159" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D159" s="35" t="s">
-        <v>386</v>
+        <v>336</v>
       </c>
       <c r="E159" s="43" t="s">
-        <v>387</v>
+        <v>337</v>
       </c>
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
@@ -10221,13 +10218,13 @@
         <v>47</v>
       </c>
       <c r="C160" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D160" s="35" t="s">
-        <v>388</v>
+        <v>338</v>
       </c>
       <c r="E160" s="43" t="s">
-        <v>389</v>
+        <v>339</v>
       </c>
       <c r="F160" s="37"/>
       <c r="G160" s="37"/>
@@ -10258,13 +10255,13 @@
         <v>47</v>
       </c>
       <c r="C161" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D161" s="35" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="E161" s="43" t="s">
-        <v>391</v>
+        <v>341</v>
       </c>
       <c r="F161" s="37"/>
       <c r="G161" s="37"/>
@@ -10295,13 +10292,13 @@
         <v>47</v>
       </c>
       <c r="C162" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D162" s="35" t="s">
-        <v>392</v>
+        <v>342</v>
       </c>
       <c r="E162" s="43" t="s">
-        <v>393</v>
+        <v>343</v>
       </c>
       <c r="F162" s="37"/>
       <c r="G162" s="37"/>
@@ -10332,13 +10329,13 @@
         <v>47</v>
       </c>
       <c r="C163" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D163" s="35" t="s">
-        <v>394</v>
+        <v>344</v>
       </c>
       <c r="E163" s="43" t="s">
-        <v>395</v>
+        <v>345</v>
       </c>
       <c r="F163" s="37"/>
       <c r="G163" s="37"/>
@@ -10369,13 +10366,13 @@
         <v>47</v>
       </c>
       <c r="C164" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D164" s="35" t="s">
-        <v>396</v>
+        <v>346</v>
       </c>
       <c r="E164" s="43" t="s">
-        <v>397</v>
+        <v>347</v>
       </c>
       <c r="F164" s="37"/>
       <c r="G164" s="37"/>
@@ -10406,13 +10403,13 @@
         <v>47</v>
       </c>
       <c r="C165" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D165" s="35" t="s">
-        <v>398</v>
+        <v>348</v>
       </c>
       <c r="E165" s="43" t="s">
-        <v>399</v>
+        <v>349</v>
       </c>
       <c r="F165" s="37"/>
       <c r="G165" s="37"/>
@@ -10446,10 +10443,10 @@
         <v>55</v>
       </c>
       <c r="D166" s="35" t="s">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="E166" s="43" t="s">
-        <v>401</v>
+        <v>351</v>
       </c>
       <c r="F166" s="37"/>
       <c r="G166" s="37"/>
@@ -10483,10 +10480,10 @@
         <v>55</v>
       </c>
       <c r="D167" s="35" t="s">
-        <v>402</v>
+        <v>352</v>
       </c>
       <c r="E167" s="43" t="s">
-        <v>403</v>
+        <v>353</v>
       </c>
       <c r="F167" s="37"/>
       <c r="G167" s="37"/>
@@ -10520,10 +10517,10 @@
         <v>48</v>
       </c>
       <c r="D168" s="35" t="s">
-        <v>404</v>
+        <v>354</v>
       </c>
       <c r="E168" s="43" t="s">
-        <v>405</v>
+        <v>355</v>
       </c>
       <c r="F168" s="37"/>
       <c r="G168" s="37"/>
@@ -10554,13 +10551,13 @@
         <v>47</v>
       </c>
       <c r="C169" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D169" s="35" t="s">
-        <v>406</v>
+        <v>356</v>
       </c>
       <c r="E169" s="43" t="s">
-        <v>407</v>
+        <v>357</v>
       </c>
       <c r="F169" s="37"/>
       <c r="G169" s="37"/>
@@ -10591,13 +10588,13 @@
         <v>47</v>
       </c>
       <c r="C170" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D170" s="35" t="s">
-        <v>408</v>
+        <v>358</v>
       </c>
       <c r="E170" s="43" t="s">
-        <v>409</v>
+        <v>359</v>
       </c>
       <c r="F170" s="37"/>
       <c r="G170" s="37"/>
@@ -10628,13 +10625,13 @@
         <v>47</v>
       </c>
       <c r="C171" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D171" s="35" t="s">
-        <v>410</v>
+        <v>360</v>
       </c>
       <c r="E171" s="43" t="s">
-        <v>411</v>
+        <v>361</v>
       </c>
       <c r="F171" s="37"/>
       <c r="G171" s="37"/>
@@ -10665,13 +10662,13 @@
         <v>47</v>
       </c>
       <c r="C172" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D172" s="35" t="s">
-        <v>412</v>
+        <v>362</v>
       </c>
       <c r="E172" s="43" t="s">
-        <v>413</v>
+        <v>363</v>
       </c>
       <c r="F172" s="37"/>
       <c r="G172" s="37"/>
@@ -10702,13 +10699,13 @@
         <v>47</v>
       </c>
       <c r="C173" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D173" s="35" t="s">
-        <v>414</v>
+        <v>364</v>
       </c>
       <c r="E173" s="43" t="s">
-        <v>415</v>
+        <v>365</v>
       </c>
       <c r="F173" s="37"/>
       <c r="G173" s="37"/>
@@ -10739,13 +10736,13 @@
         <v>47</v>
       </c>
       <c r="C174" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D174" s="35" t="s">
-        <v>416</v>
+        <v>366</v>
       </c>
       <c r="E174" s="43" t="s">
-        <v>417</v>
+        <v>367</v>
       </c>
       <c r="F174" s="37"/>
       <c r="G174" s="37"/>
@@ -10776,13 +10773,13 @@
         <v>47</v>
       </c>
       <c r="C175" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D175" s="35" t="s">
-        <v>418</v>
+        <v>368</v>
       </c>
       <c r="E175" s="43" t="s">
-        <v>419</v>
+        <v>369</v>
       </c>
       <c r="F175" s="37"/>
       <c r="G175" s="37"/>
@@ -10813,13 +10810,13 @@
         <v>47</v>
       </c>
       <c r="C176" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D176" s="35" t="s">
-        <v>420</v>
+        <v>370</v>
       </c>
       <c r="E176" s="43" t="s">
-        <v>421</v>
+        <v>371</v>
       </c>
       <c r="F176" s="35"/>
       <c r="G176" s="35"/>
@@ -10850,13 +10847,13 @@
         <v>47</v>
       </c>
       <c r="C177" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D177" s="35" t="s">
-        <v>422</v>
+        <v>372</v>
       </c>
       <c r="E177" s="43" t="s">
-        <v>423</v>
+        <v>373</v>
       </c>
       <c r="F177" s="35"/>
       <c r="G177" s="35"/>
@@ -10887,13 +10884,13 @@
         <v>47</v>
       </c>
       <c r="C178" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D178" s="35" t="s">
-        <v>424</v>
+        <v>374</v>
       </c>
       <c r="E178" s="43" t="s">
-        <v>425</v>
+        <v>375</v>
       </c>
       <c r="F178" s="35"/>
       <c r="G178" s="35"/>
@@ -10924,13 +10921,13 @@
         <v>47</v>
       </c>
       <c r="C179" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D179" s="35" t="s">
-        <v>426</v>
+        <v>376</v>
       </c>
       <c r="E179" s="43" t="s">
-        <v>427</v>
+        <v>377</v>
       </c>
       <c r="F179" s="35"/>
       <c r="G179" s="35"/>
@@ -10961,13 +10958,13 @@
         <v>47</v>
       </c>
       <c r="C180" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D180" s="35" t="s">
-        <v>428</v>
+        <v>378</v>
       </c>
       <c r="E180" s="43" t="s">
-        <v>429</v>
+        <v>379</v>
       </c>
       <c r="F180" s="35"/>
       <c r="G180" s="35"/>
@@ -11001,10 +10998,10 @@
         <v>48</v>
       </c>
       <c r="D181" s="35" t="s">
-        <v>430</v>
+        <v>380</v>
       </c>
       <c r="E181" s="44" t="s">
-        <v>431</v>
+        <v>381</v>
       </c>
       <c r="F181" s="35"/>
       <c r="G181" s="35"/>
@@ -11038,10 +11035,10 @@
         <v>55</v>
       </c>
       <c r="D182" s="35" t="s">
-        <v>432</v>
+        <v>382</v>
       </c>
       <c r="E182" s="43" t="s">
-        <v>433</v>
+        <v>383</v>
       </c>
       <c r="F182" s="35"/>
       <c r="G182" s="35"/>
@@ -11072,13 +11069,13 @@
         <v>47</v>
       </c>
       <c r="C183" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D183" s="35" t="s">
-        <v>434</v>
+        <v>384</v>
       </c>
       <c r="E183" s="43" t="s">
-        <v>435</v>
+        <v>385</v>
       </c>
       <c r="F183" s="35"/>
       <c r="G183" s="35"/>
@@ -11112,53 +11109,53 @@
         <v>57</v>
       </c>
       <c r="D184" s="35" t="s">
-        <v>436</v>
+        <v>386</v>
       </c>
       <c r="E184" s="43" t="s">
-        <v>437</v>
-      </c>
-      <c r="F184" s="35" t="s">
-        <v>59</v>
+        <v>387</v>
+      </c>
+      <c r="F184" s="60">
+        <v>46048</v>
       </c>
       <c r="G184" s="35" t="s">
-        <v>438</v>
+        <v>519</v>
       </c>
       <c r="H184" s="35" t="s">
-        <v>439</v>
+        <v>520</v>
       </c>
       <c r="I184" s="35" t="s">
-        <v>440</v>
+        <v>521</v>
       </c>
       <c r="J184" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K184" s="38"/>
       <c r="L184" s="35"/>
       <c r="M184" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N184" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O184" s="35" t="s">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="P184" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="Q184" s="38" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="R184" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S184" s="47" t="s">
-        <v>507</v>
+        <v>445</v>
       </c>
       <c r="T184" s="35"/>
       <c r="U184" s="35"/>
       <c r="V184" s="35" t="s">
-        <v>526</v>
+        <v>464</v>
       </c>
       <c r="W184" s="35" t="s">
         <v>54</v>
@@ -11172,13 +11169,13 @@
         <v>47</v>
       </c>
       <c r="C185" s="41" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="D185" s="35" t="s">
-        <v>441</v>
+        <v>388</v>
       </c>
       <c r="E185" s="43" t="s">
-        <v>442</v>
+        <v>389</v>
       </c>
       <c r="F185" s="35"/>
       <c r="G185" s="35"/>
@@ -11209,13 +11206,13 @@
         <v>47</v>
       </c>
       <c r="C186" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D186" s="35" t="s">
-        <v>443</v>
+        <v>390</v>
       </c>
       <c r="E186" s="43" t="s">
-        <v>444</v>
+        <v>391</v>
       </c>
       <c r="F186" s="37"/>
       <c r="G186" s="37"/>
@@ -11246,13 +11243,13 @@
         <v>47</v>
       </c>
       <c r="C187" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D187" s="35" t="s">
-        <v>445</v>
+        <v>392</v>
       </c>
       <c r="E187" s="43" t="s">
-        <v>446</v>
+        <v>393</v>
       </c>
       <c r="F187" s="37"/>
       <c r="G187" s="37"/>
@@ -11286,10 +11283,10 @@
         <v>48</v>
       </c>
       <c r="D188" s="41" t="s">
-        <v>447</v>
+        <v>394</v>
       </c>
       <c r="E188" s="43" t="s">
-        <v>448</v>
+        <v>395</v>
       </c>
       <c r="F188" s="37"/>
       <c r="G188" s="37"/>
@@ -11320,13 +11317,13 @@
         <v>47</v>
       </c>
       <c r="C189" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D189" s="35" t="s">
-        <v>449</v>
+        <v>396</v>
       </c>
       <c r="E189" s="43" t="s">
-        <v>450</v>
+        <v>397</v>
       </c>
       <c r="F189" s="37"/>
       <c r="G189" s="37"/>
@@ -11357,13 +11354,13 @@
         <v>47</v>
       </c>
       <c r="C190" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D190" s="35" t="s">
-        <v>451</v>
+        <v>398</v>
       </c>
       <c r="E190" s="43" t="s">
-        <v>452</v>
+        <v>399</v>
       </c>
       <c r="F190" s="37"/>
       <c r="G190" s="37"/>
@@ -11397,25 +11394,25 @@
         <v>57</v>
       </c>
       <c r="D191" s="35" t="s">
-        <v>453</v>
+        <v>400</v>
       </c>
       <c r="E191" s="43" t="s">
-        <v>454</v>
-      </c>
-      <c r="F191" s="37" t="s">
-        <v>59</v>
+        <v>401</v>
+      </c>
+      <c r="F191" s="60">
+        <v>46048</v>
       </c>
       <c r="G191" s="37" t="s">
-        <v>455</v>
+        <v>522</v>
       </c>
       <c r="H191" s="37" t="s">
-        <v>456</v>
+        <v>525</v>
       </c>
       <c r="I191" s="42" t="s">
-        <v>457</v>
+        <v>526</v>
       </c>
       <c r="J191" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K191" s="38"/>
       <c r="L191" s="38"/>
@@ -11429,7 +11426,7 @@
       <c r="T191" s="38"/>
       <c r="U191" s="39"/>
       <c r="V191" s="40" t="s">
-        <v>527</v>
+        <v>465</v>
       </c>
       <c r="W191" s="38" t="s">
         <v>51</v>
@@ -11446,25 +11443,25 @@
         <v>57</v>
       </c>
       <c r="D192" s="35" t="s">
-        <v>458</v>
+        <v>402</v>
       </c>
       <c r="E192" s="43" t="s">
-        <v>459</v>
-      </c>
-      <c r="F192" s="37" t="s">
-        <v>59</v>
+        <v>403</v>
+      </c>
+      <c r="F192" s="60">
+        <v>46048</v>
       </c>
       <c r="G192" s="37" t="s">
-        <v>460</v>
+        <v>527</v>
       </c>
       <c r="H192" s="37" t="s">
-        <v>461</v>
+        <v>523</v>
       </c>
       <c r="I192" s="42" t="s">
-        <v>462</v>
+        <v>524</v>
       </c>
       <c r="J192" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K192" s="38"/>
       <c r="L192" s="38"/>
@@ -11478,7 +11475,7 @@
       <c r="T192" s="38"/>
       <c r="U192" s="39"/>
       <c r="V192" s="40" t="s">
-        <v>528</v>
+        <v>466</v>
       </c>
       <c r="W192" s="38" t="s">
         <v>51</v>
@@ -11495,25 +11492,25 @@
         <v>57</v>
       </c>
       <c r="D193" s="35" t="s">
-        <v>463</v>
+        <v>404</v>
       </c>
       <c r="E193" s="45" t="s">
-        <v>464</v>
-      </c>
-      <c r="F193" s="37" t="s">
-        <v>59</v>
+        <v>405</v>
+      </c>
+      <c r="F193" s="60">
+        <v>46048</v>
       </c>
       <c r="G193" s="37" t="s">
-        <v>465</v>
+        <v>528</v>
       </c>
       <c r="H193" s="37" t="s">
-        <v>466</v>
+        <v>529</v>
       </c>
       <c r="I193" s="42" t="s">
-        <v>467</v>
+        <v>530</v>
       </c>
       <c r="J193" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K193" s="38"/>
       <c r="L193" s="38"/>
@@ -11527,7 +11524,7 @@
       <c r="T193" s="38"/>
       <c r="U193" s="39"/>
       <c r="V193" s="40" t="s">
-        <v>527</v>
+        <v>465</v>
       </c>
       <c r="W193" s="38" t="s">
         <v>51</v>
@@ -15519,42 +15516,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>468</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>469</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>470</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>471</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>472</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>473</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>474</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>475</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -15584,22 +15581,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" thickBot="1">
       <c r="A1" s="29" t="s">
-        <v>476</v>
+        <v>414</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>477</v>
+        <v>415</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>478</v>
+        <v>416</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>479</v>
+        <v>417</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>480</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1">
@@ -15607,13 +15604,13 @@
         <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>481</v>
+        <v>419</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>482</v>
+        <v>420</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>483</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1">
@@ -15621,83 +15618,83 @@
         <v>55</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>481</v>
+        <v>419</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>484</v>
+        <v>422</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>485</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>481</v>
+        <v>419</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>486</v>
+        <v>424</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>487</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>481</v>
+        <v>419</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>488</v>
+        <v>426</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>489</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>481</v>
+        <v>419</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>490</v>
+        <v>428</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>491</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>481</v>
+        <v>419</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>492</v>
+        <v>430</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>493</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>481</v>
+        <v>419</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>494</v>
+        <v>432</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>495</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -15705,41 +15702,41 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>481</v>
+        <v>419</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>496</v>
+        <v>434</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>497</v>
+        <v>435</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>498</v>
+        <v>436</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>481</v>
+        <v>419</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>499</v>
+        <v>437</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>500</v>
+        <v>438</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>481</v>
+        <v>419</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>501</v>
+        <v>439</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>502</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1">
@@ -16725,18 +16722,18 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>503</v>
+        <v>441</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>504</v>
+        <v>442</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>